<commit_message>
Minor correction in code question
</commit_message>
<xml_diff>
--- a/data/ICIP_V22.xlsx
+++ b/data/ICIP_V22.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jumora\Departamento Nacional de Planeacion\Equipo de Innovación Pública - DNP - Documentos\2019\00 Carpetas personales\Julian Mora\Indice\Versiones ICIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LcmayorquinL\OneDrive - Departamento Nacional de Planeacion\DIDE\2019\Data Science Projects\Innovation-Index-Algorithms\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="433" documentId="8_{CC960899-6866-4B2F-B3B9-BA0A90F8BE00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{37F69C79-894E-4B7E-9535-F4C11ACF7908}"/>
+  <xr:revisionPtr revIDLastSave="434" documentId="8_{CC960899-6866-4B2F-B3B9-BA0A90F8BE00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{608FD344-71C0-419C-B94F-8AA58D12018E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{A5D47138-5893-426C-AD9F-67A377940D13}"/>
+    <workbookView xWindow="3720" yWindow="3540" windowWidth="16200" windowHeight="9360" xr2:uid="{A5D47138-5893-426C-AD9F-67A377940D13}"/>
   </bookViews>
   <sheets>
     <sheet name="Las personas importan" sheetId="1" r:id="rId1"/>
@@ -164,9 +164,6 @@
 c. Se promovieron programas de formación</t>
   </si>
   <si>
-    <t>C05.c</t>
-  </si>
-  <si>
     <t>El aprendizaje es poder</t>
   </si>
   <si>
@@ -1152,6 +1149,9 @@
   </si>
   <si>
     <t>I+D</t>
+  </si>
+  <si>
+    <t>C05c</t>
   </si>
 </sst>
 </file>
@@ -1572,6 +1572,18 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1596,6 +1608,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1608,12 +1626,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1640,18 +1652,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1972,8 +1972,8 @@
   </sheetPr>
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,7 +1996,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -2026,34 +2026,34 @@
         <v>8</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="25" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
-        <v>187</v>
+      <c r="A2" s="92" t="s">
+        <v>186</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="94" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="94"/>
+      <c r="D2" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="113" t="s">
+      <c r="E2" s="90" t="s">
+        <v>275</v>
+      </c>
+      <c r="F2" s="98" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" s="102" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="64" t="s">
         <v>276</v>
-      </c>
-      <c r="F2" s="94" t="s">
-        <v>273</v>
-      </c>
-      <c r="G2" s="96" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="64" t="s">
-        <v>277</v>
       </c>
       <c r="I2" s="66" t="s">
         <v>20</v>
@@ -2062,29 +2062,29 @@
         <v>21</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>17</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
+      <c r="A3" s="93"/>
       <c r="B3" s="56" t="s">
-        <v>208</v>
-      </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="113" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="95"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="90" t="s">
+        <v>275</v>
+      </c>
+      <c r="F3" s="98"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="55" t="s">
         <v>276</v>
-      </c>
-      <c r="F3" s="94"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="55" t="s">
-        <v>277</v>
       </c>
       <c r="I3" s="42" t="s">
         <v>10</v>
@@ -2101,23 +2101,23 @@
       <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
+      <c r="A4" s="93"/>
       <c r="B4" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="95"/>
+      <c r="D4" s="96" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="88" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" s="96" t="s">
+        <v>273</v>
+      </c>
+      <c r="G4" s="103"/>
+      <c r="H4" s="55" t="s">
         <v>208</v>
-      </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="92" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="111" t="s">
-        <v>210</v>
-      </c>
-      <c r="F4" s="92" t="s">
-        <v>274</v>
-      </c>
-      <c r="G4" s="97"/>
-      <c r="H4" s="55" t="s">
-        <v>209</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>13</v>
@@ -2126,27 +2126,27 @@
         <v>24</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:14" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="95"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="88" t="s">
+        <v>209</v>
+      </c>
+      <c r="F5" s="99"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="55" t="s">
         <v>208</v>
-      </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="111" t="s">
-        <v>210</v>
-      </c>
-      <c r="F5" s="95"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="55" t="s">
-        <v>209</v>
       </c>
       <c r="I5" s="51" t="s">
         <v>10</v>
@@ -2155,33 +2155,33 @@
         <v>11</v>
       </c>
       <c r="K5" s="50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L5" s="51" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="132" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
+      <c r="A6" s="93"/>
       <c r="B6" s="56" t="s">
-        <v>208</v>
-      </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="92" t="s">
-        <v>186</v>
-      </c>
-      <c r="E6" s="111" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="95"/>
+      <c r="D6" s="96" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="88" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96" t="s">
+        <v>193</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>211</v>
-      </c>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92" t="s">
-        <v>194</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>212</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>13</v>
@@ -2190,27 +2190,27 @@
         <v>24</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
+      <c r="A7" s="93"/>
       <c r="B7" s="58"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="111" t="s">
+      <c r="C7" s="95"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="88" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" s="97"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="57" t="s">
         <v>211</v>
-      </c>
-      <c r="F7" s="93"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="57" t="s">
-        <v>212</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>13</v>
@@ -2219,29 +2219,29 @@
         <v>24</v>
       </c>
       <c r="K7" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="L7" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="L7" s="11" t="s">
-        <v>215</v>
-      </c>
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="89"/>
+      <c r="A8" s="93"/>
       <c r="B8" s="56" t="s">
-        <v>208</v>
-      </c>
-      <c r="C8" s="91"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="111" t="s">
-        <v>211</v>
-      </c>
-      <c r="F8" s="93"/>
-      <c r="G8" s="97" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="95"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="88" t="s">
+        <v>210</v>
+      </c>
+      <c r="F8" s="97"/>
+      <c r="G8" s="103" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>13</v>
@@ -2250,7 +2250,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>26</v>
+        <v>285</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>25</v>
@@ -2258,19 +2258,19 @@
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="89"/>
+      <c r="A9" s="93"/>
       <c r="B9" s="56" t="s">
-        <v>208</v>
-      </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="111" t="s">
-        <v>211</v>
-      </c>
-      <c r="F9" s="93"/>
-      <c r="G9" s="98"/>
+        <v>207</v>
+      </c>
+      <c r="C9" s="95"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="88" t="s">
+        <v>210</v>
+      </c>
+      <c r="F9" s="97"/>
+      <c r="G9" s="104"/>
       <c r="H9" s="55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I9" s="51" t="s">
         <v>13</v>
@@ -2279,28 +2279,28 @@
         <v>24</v>
       </c>
       <c r="K9" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="L9" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="L9" s="51" t="s">
-        <v>192</v>
-      </c>
       <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="89"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="92" t="s">
+      <c r="A10" s="93"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="96" t="s">
+        <v>260</v>
+      </c>
+      <c r="E10" s="89" t="s">
         <v>261</v>
       </c>
-      <c r="E10" s="112" t="s">
+      <c r="F10" s="100"/>
+      <c r="G10" s="96" t="s">
+        <v>169</v>
+      </c>
+      <c r="H10" s="100" t="s">
         <v>262</v>
-      </c>
-      <c r="F10" s="100"/>
-      <c r="G10" s="92" t="s">
-        <v>170</v>
-      </c>
-      <c r="H10" s="100" t="s">
-        <v>263</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>13</v>
@@ -2309,25 +2309,25 @@
         <v>24</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L10" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M10" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="330" x14ac:dyDescent="0.25">
-      <c r="A11" s="89"/>
-      <c r="C11" s="91"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="112" t="s">
-        <v>262</v>
+      <c r="A11" s="93"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="89" t="s">
+        <v>261</v>
       </c>
       <c r="F11" s="101"/>
-      <c r="G11" s="95"/>
+      <c r="G11" s="99"/>
       <c r="H11" s="101"/>
       <c r="I11" s="60" t="s">
         <v>10</v>
@@ -2377,8 +2377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FF0712-C92A-4192-9221-64C724CB252A}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E19"/>
+    <sheetView topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2426,39 +2426,39 @@
         <v>7</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K1" s="37" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="257.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="102" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="96" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="92" t="s">
+      <c r="C2" s="96" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="92" t="s">
-        <v>50</v>
+      <c r="F2" s="96" t="s">
+        <v>49</v>
       </c>
       <c r="G2" s="72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>10</v>
@@ -2467,27 +2467,27 @@
         <v>11</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="96"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
+      <c r="A3" s="102"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
       <c r="G3" s="72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>10</v>
@@ -2496,27 +2496,27 @@
         <v>11</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E4" s="93"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="111" t="s">
-        <v>218</v>
+      <c r="A4" s="102"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="97"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="88" t="s">
+        <v>217</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>10</v>
@@ -2525,29 +2525,29 @@
         <v>11</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E5" s="93"/>
-      <c r="F5" s="94" t="s">
-        <v>58</v>
+      <c r="A5" s="102"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" s="97"/>
+      <c r="F5" s="98" t="s">
+        <v>57</v>
       </c>
       <c r="G5" s="72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>10</v>
@@ -2556,29 +2556,29 @@
         <v>11</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="96"/>
-      <c r="B6" s="96"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E6" s="93"/>
-      <c r="F6" s="94"/>
+      <c r="A6" s="102"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" s="97"/>
+      <c r="F6" s="98"/>
       <c r="G6" s="72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>10</v>
@@ -2587,27 +2587,27 @@
         <v>11</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="96"/>
-      <c r="B7" s="96"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E7" s="93"/>
-      <c r="F7" s="94"/>
+      <c r="A7" s="102"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E7" s="97"/>
+      <c r="F7" s="98"/>
       <c r="G7" s="72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>10</v>
@@ -2616,27 +2616,27 @@
         <v>11</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="96"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E8" s="93"/>
-      <c r="F8" s="94"/>
+      <c r="A8" s="102"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>10</v>
@@ -2645,29 +2645,29 @@
         <v>11</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="96"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E9" s="93"/>
-      <c r="F9" s="94" t="s">
-        <v>29</v>
+      <c r="A9" s="102"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="97"/>
+      <c r="F9" s="98" t="s">
+        <v>28</v>
       </c>
       <c r="G9" s="72" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>10</v>
@@ -2676,29 +2676,29 @@
         <v>11</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="96"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E10" s="93"/>
-      <c r="F10" s="94"/>
+      <c r="A10" s="102"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
       <c r="G10" s="72" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>10</v>
@@ -2707,27 +2707,27 @@
         <v>11</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="A11" s="96"/>
-      <c r="B11" s="96"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E11" s="93"/>
-      <c r="F11" s="94"/>
+      <c r="A11" s="102"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
       <c r="G11" s="72" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>10</v>
@@ -2736,27 +2736,27 @@
         <v>11</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13" ht="255" x14ac:dyDescent="0.25">
-      <c r="A12" s="96"/>
-      <c r="B12" s="96"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E12" s="93"/>
-      <c r="F12" s="94"/>
+      <c r="A12" s="102"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E12" s="97"/>
+      <c r="F12" s="98"/>
       <c r="G12" s="72" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>10</v>
@@ -2765,204 +2765,204 @@
         <v>11</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="96"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E13" s="93"/>
-      <c r="F13" s="94" t="s">
-        <v>178</v>
+      <c r="A13" s="102"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E13" s="97"/>
+      <c r="F13" s="98" t="s">
+        <v>177</v>
       </c>
       <c r="G13" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="H13" s="94" t="s">
+        <v>220</v>
+      </c>
+      <c r="H13" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="94" t="s">
+      <c r="I13" s="98" t="s">
         <v>11</v>
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="L13" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="M13" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="96"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="93"/>
-      <c r="F14" s="94"/>
+      <c r="A14" s="102"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E14" s="97"/>
+      <c r="F14" s="98"/>
       <c r="G14" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
+        <v>220</v>
+      </c>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
       <c r="J14" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="L14" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="K14" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="96"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E15" s="93"/>
-      <c r="F15" s="94"/>
+      <c r="A15" s="102"/>
+      <c r="B15" s="102"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="H15" s="94"/>
-      <c r="I15" s="94"/>
+        <v>220</v>
+      </c>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
       <c r="J15" s="24"/>
       <c r="K15" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="96"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E16" s="93"/>
-      <c r="F16" s="94"/>
+      <c r="A16" s="102"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E16" s="97"/>
+      <c r="F16" s="98"/>
       <c r="G16" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="H16" s="94"/>
-      <c r="I16" s="94"/>
+        <v>220</v>
+      </c>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
       <c r="J16" s="24"/>
       <c r="K16" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="96"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E17" s="93"/>
-      <c r="F17" s="94"/>
+      <c r="A17" s="102"/>
+      <c r="B17" s="102"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" s="97"/>
+      <c r="F17" s="98"/>
       <c r="G17" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="H17" s="94"/>
-      <c r="I17" s="94"/>
+        <v>220</v>
+      </c>
+      <c r="H17" s="98"/>
+      <c r="I17" s="98"/>
       <c r="J17" s="24"/>
       <c r="K17" s="40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="96"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E18" s="93"/>
-      <c r="F18" s="94"/>
+      <c r="A18" s="102"/>
+      <c r="B18" s="102"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E18" s="97"/>
+      <c r="F18" s="98"/>
       <c r="G18" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="H18" s="94"/>
-      <c r="I18" s="94"/>
+        <v>220</v>
+      </c>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
       <c r="J18" s="24"/>
       <c r="K18" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="96"/>
-      <c r="B19" s="96"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="111" t="s">
-        <v>226</v>
-      </c>
-      <c r="E19" s="95"/>
-      <c r="F19" s="94"/>
+      <c r="A19" s="102"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="E19" s="99"/>
+      <c r="F19" s="98"/>
       <c r="G19" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="H19" s="94"/>
-      <c r="I19" s="94"/>
+        <v>220</v>
+      </c>
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
       <c r="J19" s="49"/>
       <c r="K19" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M19" s="28"/>
     </row>
     <row r="20" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A20" s="96"/>
-      <c r="B20" s="96"/>
-      <c r="C20" s="102" t="s">
-        <v>278</v>
+      <c r="A20" s="102"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="106" t="s">
+        <v>277</v>
       </c>
       <c r="D20" s="72" t="s">
-        <v>225</v>
-      </c>
-      <c r="E20" s="96" t="s">
-        <v>258</v>
-      </c>
-      <c r="F20" s="92" t="s">
-        <v>30</v>
+        <v>224</v>
+      </c>
+      <c r="E20" s="102" t="s">
+        <v>257</v>
+      </c>
+      <c r="F20" s="96" t="s">
+        <v>29</v>
       </c>
       <c r="G20" s="72" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H20" s="66" t="s">
         <v>10</v>
@@ -2971,27 +2971,27 @@
         <v>11</v>
       </c>
       <c r="J20" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="L20" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="K20" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="M20" s="9"/>
     </row>
     <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="96"/>
-      <c r="B21" s="96"/>
-      <c r="C21" s="102"/>
+      <c r="A21" s="102"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="106"/>
       <c r="D21" s="72" t="s">
-        <v>225</v>
-      </c>
-      <c r="E21" s="96"/>
-      <c r="F21" s="93"/>
+        <v>224</v>
+      </c>
+      <c r="E21" s="102"/>
+      <c r="F21" s="97"/>
       <c r="G21" s="72" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H21" s="46" t="s">
         <v>10</v>
@@ -3000,27 +3000,27 @@
         <v>11</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M21" s="9"/>
     </row>
     <row r="22" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="96"/>
-      <c r="B22" s="96"/>
-      <c r="C22" s="102"/>
+      <c r="A22" s="102"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="106"/>
       <c r="D22" s="72" t="s">
-        <v>225</v>
-      </c>
-      <c r="E22" s="96"/>
-      <c r="F22" s="93"/>
+        <v>224</v>
+      </c>
+      <c r="E22" s="102"/>
+      <c r="F22" s="97"/>
       <c r="G22" s="72" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H22" s="46" t="s">
         <v>10</v>
@@ -3029,27 +3029,27 @@
         <v>11</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="96"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="102"/>
+      <c r="A23" s="102"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="106"/>
       <c r="D23" s="72" t="s">
-        <v>225</v>
-      </c>
-      <c r="E23" s="96"/>
-      <c r="F23" s="93"/>
+        <v>224</v>
+      </c>
+      <c r="E23" s="102"/>
+      <c r="F23" s="97"/>
       <c r="G23" s="72" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H23" s="46" t="s">
         <v>10</v>
@@ -3061,26 +3061,26 @@
         <v>238</v>
       </c>
       <c r="K23" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="L23" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="L23" s="22" t="s">
-        <v>92</v>
-      </c>
       <c r="M23" s="9"/>
     </row>
     <row r="24" spans="1:13" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="96"/>
-      <c r="B24" s="96"/>
-      <c r="C24" s="102"/>
+      <c r="A24" s="102"/>
+      <c r="B24" s="102"/>
+      <c r="C24" s="106"/>
       <c r="D24" s="72" t="s">
-        <v>225</v>
-      </c>
-      <c r="E24" s="96"/>
-      <c r="F24" s="92" t="s">
+        <v>224</v>
+      </c>
+      <c r="E24" s="102"/>
+      <c r="F24" s="96" t="s">
+        <v>278</v>
+      </c>
+      <c r="G24" s="72" t="s">
         <v>279</v>
-      </c>
-      <c r="G24" s="72" t="s">
-        <v>280</v>
       </c>
       <c r="H24" s="46" t="s">
         <v>10</v>
@@ -3089,27 +3089,27 @@
         <v>11</v>
       </c>
       <c r="J24" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="K24" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="K24" s="18" t="s">
-        <v>83</v>
-      </c>
       <c r="L24" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:13" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="96"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="102"/>
+      <c r="A25" s="102"/>
+      <c r="B25" s="102"/>
+      <c r="C25" s="106"/>
       <c r="D25" s="72" t="s">
-        <v>225</v>
-      </c>
-      <c r="E25" s="96"/>
-      <c r="F25" s="95"/>
+        <v>224</v>
+      </c>
+      <c r="E25" s="102"/>
+      <c r="F25" s="99"/>
       <c r="G25" s="72" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>10</v>
@@ -3118,119 +3118,119 @@
         <v>11</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M25" s="9"/>
     </row>
     <row r="26" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A26" s="96"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="102" t="s">
+      <c r="A26" s="102"/>
+      <c r="B26" s="102"/>
+      <c r="C26" s="106" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="72" t="s">
+        <v>223</v>
+      </c>
+      <c r="E26" s="102" t="s">
+        <v>176</v>
+      </c>
+      <c r="F26" s="107"/>
+      <c r="G26" s="72" t="s">
+        <v>222</v>
+      </c>
+      <c r="H26" s="98" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="M26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E26" s="96" t="s">
-        <v>177</v>
-      </c>
-      <c r="F26" s="103"/>
-      <c r="G26" s="72" t="s">
+    </row>
+    <row r="27" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="102"/>
+      <c r="B27" s="102"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="72" t="s">
         <v>223</v>
       </c>
-      <c r="H26" s="94" t="s">
-        <v>10</v>
-      </c>
-      <c r="I26" s="94" t="s">
-        <v>11</v>
-      </c>
-      <c r="J26" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="K26" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="L26" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="M26" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="96"/>
-      <c r="B27" s="96"/>
-      <c r="C27" s="102"/>
-      <c r="D27" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E27" s="96"/>
-      <c r="F27" s="104"/>
+      <c r="E27" s="102"/>
+      <c r="F27" s="108"/>
       <c r="G27" s="72" t="s">
-        <v>223</v>
-      </c>
-      <c r="H27" s="94"/>
-      <c r="I27" s="94"/>
+        <v>222</v>
+      </c>
+      <c r="H27" s="98"/>
+      <c r="I27" s="98"/>
       <c r="J27" s="24"/>
       <c r="K27" s="38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M27" s="9"/>
     </row>
     <row r="28" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="96"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="102"/>
+      <c r="A28" s="102"/>
+      <c r="B28" s="102"/>
+      <c r="C28" s="106"/>
       <c r="D28" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E28" s="96"/>
-      <c r="F28" s="104"/>
+        <v>223</v>
+      </c>
+      <c r="E28" s="102"/>
+      <c r="F28" s="108"/>
       <c r="G28" s="72" t="s">
-        <v>223</v>
-      </c>
-      <c r="H28" s="94"/>
-      <c r="I28" s="94"/>
+        <v>222</v>
+      </c>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
       <c r="J28" s="24"/>
       <c r="K28" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M28" s="9"/>
     </row>
     <row r="29" spans="1:13" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="96"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="102"/>
+      <c r="A29" s="102"/>
+      <c r="B29" s="102"/>
+      <c r="C29" s="106"/>
       <c r="D29" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E29" s="96"/>
-      <c r="F29" s="105"/>
+        <v>223</v>
+      </c>
+      <c r="E29" s="102"/>
+      <c r="F29" s="109"/>
       <c r="G29" s="72" t="s">
-        <v>223</v>
-      </c>
-      <c r="H29" s="94"/>
-      <c r="I29" s="94"/>
+        <v>222</v>
+      </c>
+      <c r="H29" s="98"/>
+      <c r="I29" s="98"/>
       <c r="J29" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M29" s="9"/>
     </row>
@@ -3275,7 +3275,7 @@
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="114" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="91" customWidth="1"/>
     <col min="5" max="5" width="51.42578125" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
@@ -3315,39 +3315,39 @@
         <v>7</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K1" s="37" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="14" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="C2" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="92" t="s">
-        <v>115</v>
-      </c>
       <c r="D2" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" s="96" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="96" t="s">
+        <v>181</v>
+      </c>
+      <c r="G2" s="70" t="s">
         <v>227</v>
-      </c>
-      <c r="E2" s="92" t="s">
-        <v>181</v>
-      </c>
-      <c r="F2" s="92" t="s">
-        <v>182</v>
-      </c>
-      <c r="G2" s="70" t="s">
-        <v>228</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>13</v>
@@ -3357,24 +3357,24 @@
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" s="14" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="98"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="93"/>
+      <c r="A3" s="104"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="97"/>
       <c r="D3" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="70" t="s">
         <v>227</v>
-      </c>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="70" t="s">
-        <v>228</v>
       </c>
       <c r="H3" s="59" t="s">
         <v>13</v>
@@ -3384,24 +3384,24 @@
       </c>
       <c r="J3" s="66"/>
       <c r="K3" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L3" s="66" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" s="14" customFormat="1" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="98"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="93"/>
+      <c r="A4" s="104"/>
+      <c r="B4" s="104"/>
+      <c r="C4" s="97"/>
       <c r="D4" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="70" t="s">
         <v>227</v>
-      </c>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="70" t="s">
-        <v>228</v>
       </c>
       <c r="H4" s="15" t="s">
         <v>10</v>
@@ -3410,27 +3410,27 @@
         <v>11</v>
       </c>
       <c r="J4" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K4" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="K4" s="18" t="s">
-        <v>119</v>
-      </c>
       <c r="L4" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M4" s="26"/>
     </row>
     <row r="5" spans="1:13" s="14" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="98"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="93"/>
+      <c r="A5" s="104"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="97"/>
       <c r="D5" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="70" t="s">
         <v>227</v>
-      </c>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="70" t="s">
-        <v>228</v>
       </c>
       <c r="H5" s="21" t="s">
         <v>10</v>
@@ -3439,27 +3439,27 @@
         <v>11</v>
       </c>
       <c r="J5" s="86" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="L5" s="87" t="s">
-        <v>89</v>
-      </c>
       <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" s="14" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="98"/>
-      <c r="B6" s="98"/>
-      <c r="C6" s="93"/>
+      <c r="A6" s="104"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="97"/>
       <c r="D6" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="70" t="s">
         <v>227</v>
-      </c>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="70" t="s">
-        <v>228</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>10</v>
@@ -3471,24 +3471,24 @@
         <v>216</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:13" s="14" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="98"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="93"/>
+      <c r="A7" s="104"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="97"/>
       <c r="D7" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="70" t="s">
         <v>227</v>
-      </c>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="70" t="s">
-        <v>228</v>
       </c>
       <c r="H7" s="59" t="s">
         <v>13</v>
@@ -3498,24 +3498,24 @@
       </c>
       <c r="J7" s="58"/>
       <c r="K7" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" s="14" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="98"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="93"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="97"/>
       <c r="D8" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="70" t="s">
         <v>227</v>
-      </c>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="70" t="s">
-        <v>228</v>
       </c>
       <c r="H8" s="59" t="s">
         <v>13</v>
@@ -3525,24 +3525,24 @@
       </c>
       <c r="J8" s="59"/>
       <c r="K8" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" s="14" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="98"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="93"/>
+      <c r="A9" s="104"/>
+      <c r="B9" s="104"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="70" t="s">
         <v>227</v>
-      </c>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="70" t="s">
-        <v>228</v>
       </c>
       <c r="H9" s="15" t="s">
         <v>10</v>
@@ -3554,26 +3554,26 @@
         <v>225</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="98"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="93"/>
+      <c r="A10" s="104"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="E10" s="93"/>
-      <c r="F10" s="92" t="s">
-        <v>183</v>
+        <v>226</v>
+      </c>
+      <c r="E10" s="97"/>
+      <c r="F10" s="96" t="s">
+        <v>182</v>
       </c>
       <c r="G10" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H10" s="66" t="s">
         <v>10</v>
@@ -3582,29 +3582,29 @@
         <v>11</v>
       </c>
       <c r="J10" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="L10" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="K10" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="L10" s="23" t="s">
-        <v>126</v>
-      </c>
       <c r="M10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="98"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="93"/>
+      <c r="A11" s="104"/>
+      <c r="B11" s="104"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="E11" s="93"/>
-      <c r="F11" s="93"/>
+        <v>226</v>
+      </c>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
       <c r="G11" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H11" s="59" t="s">
         <v>13</v>
@@ -3614,24 +3614,24 @@
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M11" s="20"/>
     </row>
     <row r="12" spans="1:13" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="98"/>
-      <c r="B12" s="98"/>
-      <c r="C12" s="93"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="104"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
+        <v>226</v>
+      </c>
+      <c r="E12" s="97"/>
+      <c r="F12" s="97"/>
       <c r="G12" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H12" s="15" t="s">
         <v>10</v>
@@ -3640,27 +3640,27 @@
         <v>11</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:13" s="14" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A13" s="98"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="93"/>
+      <c r="A13" s="104"/>
+      <c r="B13" s="104"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
+        <v>226</v>
+      </c>
+      <c r="E13" s="97"/>
+      <c r="F13" s="97"/>
       <c r="G13" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>10</v>
@@ -3669,27 +3669,27 @@
         <v>11</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="98"/>
-      <c r="B14" s="98"/>
-      <c r="C14" s="93"/>
+      <c r="A14" s="104"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="97"/>
       <c r="D14" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
+        <v>226</v>
+      </c>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
       <c r="G14" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H14" s="53" t="s">
         <v>10</v>
@@ -3699,24 +3699,24 @@
       </c>
       <c r="J14" s="9"/>
       <c r="K14" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L14" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:13" s="14" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="98"/>
-      <c r="B15" s="98"/>
-      <c r="C15" s="93"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="97"/>
       <c r="D15" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="E15" s="93"/>
-      <c r="F15" s="95"/>
+        <v>226</v>
+      </c>
+      <c r="E15" s="97"/>
+      <c r="F15" s="99"/>
       <c r="G15" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>10</v>
@@ -3725,29 +3725,29 @@
         <v>11</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M15" s="9"/>
     </row>
     <row r="16" spans="1:13" s="14" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="98"/>
-      <c r="B16" s="98"/>
-      <c r="C16" s="93"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="97"/>
       <c r="D16" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="E16" s="93"/>
-      <c r="F16" s="92" t="s">
-        <v>275</v>
+        <v>226</v>
+      </c>
+      <c r="E16" s="97"/>
+      <c r="F16" s="96" t="s">
+        <v>274</v>
       </c>
       <c r="G16" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H16" s="66" t="s">
         <v>10</v>
@@ -3756,27 +3756,27 @@
         <v>11</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L16" s="67" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M16" s="9"/>
     </row>
     <row r="17" spans="1:13" s="14" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="98"/>
-      <c r="B17" s="98"/>
-      <c r="C17" s="93"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="97"/>
       <c r="D17" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
+        <v>226</v>
+      </c>
+      <c r="E17" s="97"/>
+      <c r="F17" s="97"/>
       <c r="G17" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H17" s="66" t="s">
         <v>10</v>
@@ -3785,27 +3785,27 @@
         <v>11</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L17" s="67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M17" s="9"/>
     </row>
     <row r="18" spans="1:13" s="14" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="98"/>
-      <c r="B18" s="98"/>
-      <c r="C18" s="93"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="104"/>
+      <c r="C18" s="97"/>
       <c r="D18" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
+        <v>226</v>
+      </c>
+      <c r="E18" s="97"/>
+      <c r="F18" s="97"/>
       <c r="G18" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H18" s="66" t="s">
         <v>10</v>
@@ -3814,27 +3814,27 @@
         <v>11</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K18" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="L18" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="L18" s="67" t="s">
-        <v>142</v>
-      </c>
       <c r="M18" s="9"/>
     </row>
     <row r="19" spans="1:13" s="14" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="98"/>
-      <c r="B19" s="98"/>
-      <c r="C19" s="93"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="97"/>
       <c r="D19" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
+        <v>226</v>
+      </c>
+      <c r="E19" s="97"/>
+      <c r="F19" s="97"/>
       <c r="G19" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H19" s="66" t="s">
         <v>10</v>
@@ -3844,30 +3844,30 @@
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L19" s="67" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:13" s="84" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="98"/>
-      <c r="B20" s="98"/>
-      <c r="C20" s="96" t="s">
-        <v>116</v>
+      <c r="A20" s="104"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="102" t="s">
+        <v>115</v>
       </c>
       <c r="D20" s="70" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" s="102" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" s="96" t="s">
+        <v>183</v>
+      </c>
+      <c r="G20" s="70" t="s">
         <v>231</v>
-      </c>
-      <c r="E20" s="96" t="s">
-        <v>175</v>
-      </c>
-      <c r="F20" s="92" t="s">
-        <v>184</v>
-      </c>
-      <c r="G20" s="70" t="s">
-        <v>232</v>
       </c>
       <c r="H20" s="81" t="s">
         <v>13</v>
@@ -3876,27 +3876,27 @@
         <v>24</v>
       </c>
       <c r="J20" s="82" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L20" s="83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M20" s="82"/>
     </row>
     <row r="21" spans="1:13" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="98"/>
-      <c r="B21" s="98"/>
-      <c r="C21" s="96"/>
+      <c r="A21" s="104"/>
+      <c r="B21" s="104"/>
+      <c r="C21" s="102"/>
       <c r="D21" s="70" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="102"/>
+      <c r="F21" s="97"/>
+      <c r="G21" s="70" t="s">
         <v>231</v>
-      </c>
-      <c r="E21" s="96"/>
-      <c r="F21" s="93"/>
-      <c r="G21" s="70" t="s">
-        <v>232</v>
       </c>
       <c r="H21" s="15" t="s">
         <v>13</v>
@@ -3905,27 +3905,27 @@
         <v>24</v>
       </c>
       <c r="J21" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="L21" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="K21" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="L21" s="23" t="s">
-        <v>150</v>
-      </c>
       <c r="M21" s="9"/>
     </row>
     <row r="22" spans="1:13" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="98"/>
-      <c r="B22" s="98"/>
-      <c r="C22" s="96"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="102"/>
       <c r="D22" s="70" t="s">
+        <v>230</v>
+      </c>
+      <c r="E22" s="102"/>
+      <c r="F22" s="97"/>
+      <c r="G22" s="70" t="s">
         <v>231</v>
-      </c>
-      <c r="E22" s="96"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="70" t="s">
-        <v>232</v>
       </c>
       <c r="H22" s="59" t="s">
         <v>13</v>
@@ -3935,26 +3935,26 @@
       </c>
       <c r="J22" s="24"/>
       <c r="K22" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L22" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:13" s="14" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="98"/>
-      <c r="B23" s="98"/>
-      <c r="C23" s="96"/>
+      <c r="A23" s="104"/>
+      <c r="B23" s="104"/>
+      <c r="C23" s="102"/>
       <c r="D23" s="70" t="s">
-        <v>231</v>
-      </c>
-      <c r="E23" s="96"/>
-      <c r="F23" s="94" t="s">
-        <v>173</v>
+        <v>230</v>
+      </c>
+      <c r="E23" s="102"/>
+      <c r="F23" s="98" t="s">
+        <v>172</v>
       </c>
       <c r="G23" s="70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H23" s="66" t="s">
         <v>10</v>
@@ -3964,24 +3964,24 @@
       </c>
       <c r="J23" s="24"/>
       <c r="K23" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L23" s="67" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M23" s="9"/>
     </row>
     <row r="24" spans="1:13" s="14" customFormat="1" ht="205.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="98"/>
-      <c r="B24" s="98"/>
-      <c r="C24" s="96"/>
+      <c r="A24" s="104"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="102"/>
       <c r="D24" s="70" t="s">
-        <v>231</v>
-      </c>
-      <c r="E24" s="96"/>
-      <c r="F24" s="94"/>
+        <v>230</v>
+      </c>
+      <c r="E24" s="102"/>
+      <c r="F24" s="98"/>
       <c r="G24" s="70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H24" s="66" t="s">
         <v>10</v>
@@ -3990,27 +3990,27 @@
         <v>11</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L24" s="67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M24" s="48"/>
     </row>
     <row r="25" spans="1:13" s="14" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="98"/>
-      <c r="B25" s="98"/>
-      <c r="C25" s="96"/>
+      <c r="A25" s="104"/>
+      <c r="B25" s="104"/>
+      <c r="C25" s="102"/>
       <c r="D25" s="70" t="s">
-        <v>231</v>
-      </c>
-      <c r="E25" s="96"/>
-      <c r="F25" s="94"/>
+        <v>230</v>
+      </c>
+      <c r="E25" s="102"/>
+      <c r="F25" s="98"/>
       <c r="G25" s="70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H25" s="66" t="s">
         <v>10</v>
@@ -4019,27 +4019,27 @@
         <v>11</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L25" s="67" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M25" s="48"/>
     </row>
     <row r="26" spans="1:13" s="14" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="98"/>
-      <c r="B26" s="98"/>
-      <c r="C26" s="96"/>
+      <c r="A26" s="104"/>
+      <c r="B26" s="104"/>
+      <c r="C26" s="102"/>
       <c r="D26" s="70" t="s">
-        <v>231</v>
-      </c>
-      <c r="E26" s="96"/>
-      <c r="F26" s="94"/>
+        <v>230</v>
+      </c>
+      <c r="E26" s="102"/>
+      <c r="F26" s="98"/>
       <c r="G26" s="70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H26" s="66" t="s">
         <v>13</v>
@@ -4049,24 +4049,24 @@
       </c>
       <c r="J26" s="24"/>
       <c r="K26" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L26" s="67" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M26" s="48"/>
     </row>
     <row r="27" spans="1:13" s="14" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="98"/>
-      <c r="B27" s="98"/>
-      <c r="C27" s="96"/>
+      <c r="A27" s="104"/>
+      <c r="B27" s="104"/>
+      <c r="C27" s="102"/>
       <c r="D27" s="70" t="s">
-        <v>231</v>
-      </c>
-      <c r="E27" s="96"/>
-      <c r="F27" s="94"/>
+        <v>230</v>
+      </c>
+      <c r="E27" s="102"/>
+      <c r="F27" s="98"/>
       <c r="G27" s="70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H27" s="66" t="s">
         <v>13</v>
@@ -4076,10 +4076,10 @@
       </c>
       <c r="J27" s="24"/>
       <c r="K27" s="39" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L27" s="67" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M27" s="48"/>
     </row>
@@ -4156,13 +4156,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>9</v>
@@ -4170,20 +4170,20 @@
       <c r="N1" s="28"/>
     </row>
     <row r="2" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="106" t="s">
-        <v>180</v>
-      </c>
-      <c r="B2" s="106"/>
+      <c r="A2" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="110"/>
       <c r="C2" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" s="68" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E2" s="62"/>
       <c r="F2" s="63"/>
       <c r="G2" s="68" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>13</v>
@@ -4192,13 +4192,13 @@
         <v>24</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L2" s="67" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>12</v>
@@ -4206,18 +4206,18 @@
       <c r="N2" s="28"/>
     </row>
     <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="106"/>
-      <c r="B3" s="106"/>
+      <c r="A3" s="110"/>
+      <c r="B3" s="110"/>
       <c r="C3" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="61" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E3" s="62"/>
       <c r="F3" s="32"/>
       <c r="G3" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>13</v>
@@ -4226,13 +4226,13 @@
         <v>24</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>12</v>
@@ -4240,22 +4240,22 @@
       <c r="N3" s="28"/>
     </row>
     <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="106"/>
-      <c r="B4" s="106"/>
+      <c r="A4" s="110"/>
+      <c r="B4" s="110"/>
       <c r="C4" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D4" s="61" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="33" t="s">
         <v>238</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>239</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>10</v>
@@ -4264,32 +4264,32 @@
         <v>11</v>
       </c>
       <c r="J4" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="K4" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="K4" s="29" t="s">
-        <v>154</v>
-      </c>
       <c r="L4" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="28"/>
     </row>
     <row r="5" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="109" t="s">
-        <v>271</v>
+      <c r="A5" s="110"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="113" t="s">
+        <v>270</v>
       </c>
       <c r="D5" s="71" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E5" s="63"/>
       <c r="F5" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G5" s="71" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H5" s="62" t="s">
         <v>10</v>
@@ -4298,30 +4298,30 @@
         <v>11</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="L5" s="22" t="s">
         <v>269</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>270</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="28"/>
     </row>
     <row r="6" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="106"/>
-      <c r="B6" s="106"/>
-      <c r="C6" s="110"/>
+      <c r="A6" s="110"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="114"/>
       <c r="D6" s="71" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E6" s="63"/>
       <c r="F6" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G6" s="73" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H6" s="67" t="s">
         <v>10</v>
@@ -4330,34 +4330,34 @@
         <v>11</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="28"/>
     </row>
     <row r="7" spans="1:14" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="106"/>
-      <c r="B7" s="106"/>
-      <c r="C7" s="107" t="s">
-        <v>272</v>
-      </c>
-      <c r="D7" s="108" t="s">
+      <c r="A7" s="110"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="111" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" s="112" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="112" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="112" t="s">
+        <v>158</v>
+      </c>
+      <c r="G7" s="76" t="s">
         <v>234</v>
-      </c>
-      <c r="E7" s="108" t="s">
-        <v>167</v>
-      </c>
-      <c r="F7" s="108" t="s">
-        <v>159</v>
-      </c>
-      <c r="G7" s="76" t="s">
-        <v>235</v>
       </c>
       <c r="H7" s="74" t="s">
         <v>10</v>
@@ -4367,10 +4367,10 @@
       </c>
       <c r="J7" s="75"/>
       <c r="K7" s="76" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L7" s="74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M7" s="75"/>
       <c r="N7" s="7" t="s">
@@ -4378,14 +4378,14 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="195" x14ac:dyDescent="0.25">
-      <c r="A8" s="106"/>
-      <c r="B8" s="106"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
       <c r="G8" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H8" s="77" t="s">
         <v>10</v>
@@ -4395,10 +4395,10 @@
       </c>
       <c r="J8" s="77"/>
       <c r="K8" s="78" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L8" s="79" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M8" s="80"/>
       <c r="N8" s="28"/>
@@ -4662,16 +4662,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BA4D476-32CA-4B93-8A89-8E5E8618A3F8}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="9b272e4e-2ce1-4322-a085-a85112500e72"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="57d38346-cf2b-472c-9a09-6eba75d26f5c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9b272e4e-2ce1-4322-a085-a85112500e72"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixing missing column in vector
</commit_message>
<xml_diff>
--- a/data/ICIP_V22.xlsx
+++ b/data/ICIP_V22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LcmayorquinL\OneDrive - Departamento Nacional de Planeacion\DIDE\2019\Data Science Projects\Innovation-Index-Algorithms\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="434" documentId="8_{CC960899-6866-4B2F-B3B9-BA0A90F8BE00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{608FD344-71C0-419C-B94F-8AA58D12018E}"/>
+  <xr:revisionPtr revIDLastSave="436" documentId="8_{CC960899-6866-4B2F-B3B9-BA0A90F8BE00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{1076D372-8AFB-4F0B-8550-EDF0724E8585}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="3540" windowWidth="16200" windowHeight="9360" xr2:uid="{A5D47138-5893-426C-AD9F-67A377940D13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{A5D47138-5893-426C-AD9F-67A377940D13}"/>
   </bookViews>
   <sheets>
     <sheet name="Las personas importan" sheetId="1" r:id="rId1"/>
@@ -356,9 +356,6 @@
     <t>297</t>
   </si>
   <si>
-    <t>115A;115B;115C;115D;115E;</t>
-  </si>
-  <si>
     <t>131C;131D;</t>
   </si>
   <si>
@@ -1152,6 +1149,9 @@
   </si>
   <si>
     <t>C05c</t>
+  </si>
+  <si>
+    <t>115A;115B;115C;115D;115E;115F;</t>
   </si>
 </sst>
 </file>
@@ -1584,6 +1584,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1596,47 +1620,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1972,7 +1972,7 @@
   </sheetPr>
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="G11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -1996,7 +1996,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -2033,27 +2033,27 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="25" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
-        <v>186</v>
+      <c r="A2" s="100" t="s">
+        <v>185</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="98" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="102"/>
+      <c r="D2" s="105" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="90" t="s">
+        <v>274</v>
+      </c>
+      <c r="F2" s="105" t="s">
+        <v>271</v>
+      </c>
+      <c r="G2" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="64" t="s">
         <v>275</v>
-      </c>
-      <c r="F2" s="98" t="s">
-        <v>272</v>
-      </c>
-      <c r="G2" s="102" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="64" t="s">
-        <v>276</v>
       </c>
       <c r="I2" s="66" t="s">
         <v>20</v>
@@ -2062,29 +2062,29 @@
         <v>21</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>17</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="93"/>
+      <c r="A3" s="101"/>
       <c r="B3" s="56" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="98"/>
+        <v>206</v>
+      </c>
+      <c r="C3" s="103"/>
+      <c r="D3" s="105"/>
       <c r="E3" s="90" t="s">
+        <v>274</v>
+      </c>
+      <c r="F3" s="105"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="55" t="s">
         <v>275</v>
-      </c>
-      <c r="F3" s="98"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="55" t="s">
-        <v>276</v>
       </c>
       <c r="I3" s="42" t="s">
         <v>10</v>
@@ -2101,23 +2101,23 @@
       <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="93"/>
+      <c r="A4" s="101"/>
       <c r="B4" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" s="103"/>
+      <c r="D4" s="94" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="88" t="s">
+        <v>208</v>
+      </c>
+      <c r="F4" s="94" t="s">
+        <v>272</v>
+      </c>
+      <c r="G4" s="97"/>
+      <c r="H4" s="55" t="s">
         <v>207</v>
-      </c>
-      <c r="C4" s="95"/>
-      <c r="D4" s="96" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="88" t="s">
-        <v>209</v>
-      </c>
-      <c r="F4" s="96" t="s">
-        <v>273</v>
-      </c>
-      <c r="G4" s="103"/>
-      <c r="H4" s="55" t="s">
-        <v>208</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>13</v>
@@ -2126,27 +2126,27 @@
         <v>24</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:14" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="93"/>
+      <c r="A5" s="101"/>
       <c r="B5" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="103"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="88" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" s="95"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="55" t="s">
         <v>207</v>
-      </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="88" t="s">
-        <v>209</v>
-      </c>
-      <c r="F5" s="99"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="55" t="s">
-        <v>208</v>
       </c>
       <c r="I5" s="51" t="s">
         <v>10</v>
@@ -2155,33 +2155,33 @@
         <v>11</v>
       </c>
       <c r="K5" s="50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L5" s="51" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="132" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
+      <c r="A6" s="101"/>
       <c r="B6" s="56" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="96" t="s">
-        <v>185</v>
+        <v>206</v>
+      </c>
+      <c r="C6" s="103"/>
+      <c r="D6" s="94" t="s">
+        <v>184</v>
       </c>
       <c r="E6" s="88" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96" t="s">
-        <v>193</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>13</v>
@@ -2190,27 +2190,27 @@
         <v>24</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="93"/>
+      <c r="A7" s="101"/>
       <c r="B7" s="58"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="97"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="104"/>
       <c r="E7" s="88" t="s">
+        <v>209</v>
+      </c>
+      <c r="F7" s="104"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="57" t="s">
         <v>210</v>
-      </c>
-      <c r="F7" s="97"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="57" t="s">
-        <v>211</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>13</v>
@@ -2219,29 +2219,29 @@
         <v>24</v>
       </c>
       <c r="K7" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="L7" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="L7" s="11" t="s">
-        <v>214</v>
-      </c>
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="93"/>
+      <c r="A8" s="101"/>
       <c r="B8" s="56" t="s">
-        <v>207</v>
-      </c>
-      <c r="C8" s="95"/>
-      <c r="D8" s="97"/>
+        <v>206</v>
+      </c>
+      <c r="C8" s="103"/>
+      <c r="D8" s="104"/>
       <c r="E8" s="88" t="s">
-        <v>210</v>
-      </c>
-      <c r="F8" s="97"/>
-      <c r="G8" s="103" t="s">
+        <v>209</v>
+      </c>
+      <c r="F8" s="104"/>
+      <c r="G8" s="97" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>13</v>
@@ -2250,7 +2250,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>25</v>
@@ -2258,19 +2258,19 @@
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="93"/>
+      <c r="A9" s="101"/>
       <c r="B9" s="56" t="s">
-        <v>207</v>
-      </c>
-      <c r="C9" s="95"/>
-      <c r="D9" s="97"/>
+        <v>206</v>
+      </c>
+      <c r="C9" s="103"/>
+      <c r="D9" s="104"/>
       <c r="E9" s="88" t="s">
-        <v>210</v>
-      </c>
-      <c r="F9" s="97"/>
-      <c r="G9" s="104"/>
+        <v>209</v>
+      </c>
+      <c r="F9" s="104"/>
+      <c r="G9" s="98"/>
       <c r="H9" s="55" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I9" s="51" t="s">
         <v>13</v>
@@ -2279,28 +2279,28 @@
         <v>24</v>
       </c>
       <c r="K9" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="L9" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="L9" s="51" t="s">
-        <v>191</v>
-      </c>
       <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="93"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="96" t="s">
+      <c r="A10" s="101"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="94" t="s">
+        <v>259</v>
+      </c>
+      <c r="E10" s="89" t="s">
         <v>260</v>
       </c>
-      <c r="E10" s="89" t="s">
+      <c r="F10" s="92"/>
+      <c r="G10" s="94" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="92" t="s">
         <v>261</v>
-      </c>
-      <c r="F10" s="100"/>
-      <c r="G10" s="96" t="s">
-        <v>169</v>
-      </c>
-      <c r="H10" s="100" t="s">
-        <v>262</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>13</v>
@@ -2309,26 +2309,26 @@
         <v>24</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L10" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M10" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="330" x14ac:dyDescent="0.25">
-      <c r="A11" s="93"/>
-      <c r="C11" s="95"/>
-      <c r="D11" s="99"/>
+      <c r="A11" s="101"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="95"/>
       <c r="E11" s="89" t="s">
-        <v>261</v>
-      </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="101"/>
+        <v>260</v>
+      </c>
+      <c r="F11" s="93"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="93"/>
       <c r="I11" s="60" t="s">
         <v>10</v>
       </c>
@@ -2350,6 +2350,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="F10:F11"/>
@@ -2358,14 +2366,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="27" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2377,8 +2377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FF0712-C92A-4192-9221-64C724CB252A}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:F29"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2439,26 +2439,26 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="257.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="96" t="s">
+      <c r="C2" s="94" t="s">
         <v>37</v>
       </c>
       <c r="D2" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E2" s="96" t="s">
+        <v>224</v>
+      </c>
+      <c r="E2" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="96" t="s">
+      <c r="F2" s="94" t="s">
         <v>49</v>
       </c>
       <c r="G2" s="72" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>10</v>
@@ -2478,16 +2478,16 @@
       <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="102"/>
-      <c r="B3" s="102"/>
-      <c r="C3" s="97"/>
+      <c r="A3" s="96"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="104"/>
       <c r="D3" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
+        <v>224</v>
+      </c>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
       <c r="G3" s="72" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>10</v>
@@ -2507,16 +2507,16 @@
       <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="102"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="97"/>
+      <c r="A4" s="96"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="104"/>
       <c r="D4" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E4" s="97"/>
-      <c r="F4" s="99"/>
+        <v>224</v>
+      </c>
+      <c r="E4" s="104"/>
+      <c r="F4" s="95"/>
       <c r="G4" s="88" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>10</v>
@@ -2536,18 +2536,18 @@
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="102"/>
-      <c r="B5" s="102"/>
-      <c r="C5" s="97"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="104"/>
       <c r="D5" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E5" s="97"/>
-      <c r="F5" s="98" t="s">
+        <v>224</v>
+      </c>
+      <c r="E5" s="104"/>
+      <c r="F5" s="105" t="s">
         <v>57</v>
       </c>
       <c r="G5" s="72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>10</v>
@@ -2569,16 +2569,16 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="102"/>
-      <c r="B6" s="102"/>
-      <c r="C6" s="97"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="104"/>
       <c r="D6" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E6" s="97"/>
-      <c r="F6" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E6" s="104"/>
+      <c r="F6" s="105"/>
       <c r="G6" s="72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>10</v>
@@ -2590,24 +2590,24 @@
         <v>52</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="102"/>
-      <c r="B7" s="102"/>
-      <c r="C7" s="97"/>
+      <c r="A7" s="96"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="104"/>
       <c r="D7" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E7" s="97"/>
-      <c r="F7" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E7" s="104"/>
+      <c r="F7" s="105"/>
       <c r="G7" s="72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>10</v>
@@ -2627,16 +2627,16 @@
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="102"/>
-      <c r="B8" s="102"/>
-      <c r="C8" s="97"/>
+      <c r="A8" s="96"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="104"/>
       <c r="D8" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E8" s="97"/>
-      <c r="F8" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="72" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>10</v>
@@ -2648,7 +2648,7 @@
         <v>54</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>39</v>
@@ -2656,18 +2656,18 @@
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="102"/>
-      <c r="B9" s="102"/>
-      <c r="C9" s="97"/>
+      <c r="A9" s="96"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="104"/>
       <c r="D9" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E9" s="97"/>
-      <c r="F9" s="98" t="s">
+        <v>224</v>
+      </c>
+      <c r="E9" s="104"/>
+      <c r="F9" s="105" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>10</v>
@@ -2689,16 +2689,16 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="102"/>
-      <c r="B10" s="102"/>
-      <c r="C10" s="97"/>
+      <c r="A10" s="96"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="104"/>
       <c r="D10" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E10" s="97"/>
-      <c r="F10" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E10" s="104"/>
+      <c r="F10" s="105"/>
       <c r="G10" s="72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>10</v>
@@ -2718,16 +2718,16 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="A11" s="102"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="97"/>
+      <c r="A11" s="96"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="104"/>
       <c r="D11" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E11" s="97"/>
-      <c r="F11" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E11" s="104"/>
+      <c r="F11" s="105"/>
       <c r="G11" s="72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>10</v>
@@ -2747,16 +2747,16 @@
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13" ht="255" x14ac:dyDescent="0.25">
-      <c r="A12" s="102"/>
-      <c r="B12" s="102"/>
-      <c r="C12" s="97"/>
+      <c r="A12" s="96"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="104"/>
       <c r="D12" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E12" s="97"/>
-      <c r="F12" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E12" s="104"/>
+      <c r="F12" s="105"/>
       <c r="G12" s="72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>10</v>
@@ -2776,193 +2776,193 @@
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="102"/>
-      <c r="B13" s="102"/>
-      <c r="C13" s="97"/>
+      <c r="A13" s="96"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="104"/>
       <c r="D13" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E13" s="97"/>
-      <c r="F13" s="98" t="s">
-        <v>177</v>
+        <v>224</v>
+      </c>
+      <c r="E13" s="104"/>
+      <c r="F13" s="105" t="s">
+        <v>176</v>
       </c>
       <c r="G13" s="72" t="s">
-        <v>220</v>
-      </c>
-      <c r="H13" s="98" t="s">
+        <v>219</v>
+      </c>
+      <c r="H13" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="98" t="s">
+      <c r="I13" s="105" t="s">
         <v>11</v>
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="L13" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="M13" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="102"/>
-      <c r="B14" s="102"/>
-      <c r="C14" s="97"/>
+      <c r="A14" s="96"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="104"/>
       <c r="D14" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E14" s="97"/>
-      <c r="F14" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E14" s="104"/>
+      <c r="F14" s="105"/>
       <c r="G14" s="72" t="s">
-        <v>220</v>
-      </c>
-      <c r="H14" s="98"/>
-      <c r="I14" s="98"/>
+        <v>219</v>
+      </c>
+      <c r="H14" s="105"/>
+      <c r="I14" s="105"/>
       <c r="J14" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="L14" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="K14" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>108</v>
-      </c>
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="102"/>
-      <c r="B15" s="102"/>
-      <c r="C15" s="97"/>
+      <c r="A15" s="96"/>
+      <c r="B15" s="96"/>
+      <c r="C15" s="104"/>
       <c r="D15" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="72" t="s">
-        <v>220</v>
-      </c>
-      <c r="H15" s="98"/>
-      <c r="I15" s="98"/>
+        <v>219</v>
+      </c>
+      <c r="H15" s="105"/>
+      <c r="I15" s="105"/>
       <c r="J15" s="24"/>
       <c r="K15" s="40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="102"/>
-      <c r="B16" s="102"/>
-      <c r="C16" s="97"/>
+      <c r="A16" s="96"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="104"/>
       <c r="D16" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E16" s="97"/>
-      <c r="F16" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E16" s="104"/>
+      <c r="F16" s="105"/>
       <c r="G16" s="72" t="s">
-        <v>220</v>
-      </c>
-      <c r="H16" s="98"/>
-      <c r="I16" s="98"/>
+        <v>219</v>
+      </c>
+      <c r="H16" s="105"/>
+      <c r="I16" s="105"/>
       <c r="J16" s="24"/>
       <c r="K16" s="40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="102"/>
-      <c r="B17" s="102"/>
-      <c r="C17" s="97"/>
+      <c r="A17" s="96"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="104"/>
       <c r="D17" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E17" s="97"/>
-      <c r="F17" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E17" s="104"/>
+      <c r="F17" s="105"/>
       <c r="G17" s="72" t="s">
-        <v>220</v>
-      </c>
-      <c r="H17" s="98"/>
-      <c r="I17" s="98"/>
+        <v>219</v>
+      </c>
+      <c r="H17" s="105"/>
+      <c r="I17" s="105"/>
       <c r="J17" s="24"/>
       <c r="K17" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="102"/>
-      <c r="B18" s="102"/>
-      <c r="C18" s="97"/>
+      <c r="A18" s="96"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="104"/>
       <c r="D18" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E18" s="97"/>
-      <c r="F18" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E18" s="104"/>
+      <c r="F18" s="105"/>
       <c r="G18" s="72" t="s">
-        <v>220</v>
-      </c>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
+        <v>219</v>
+      </c>
+      <c r="H18" s="105"/>
+      <c r="I18" s="105"/>
       <c r="J18" s="24"/>
       <c r="K18" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="102"/>
-      <c r="B19" s="102"/>
-      <c r="C19" s="99"/>
+      <c r="A19" s="96"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="95"/>
       <c r="D19" s="88" t="s">
-        <v>225</v>
-      </c>
-      <c r="E19" s="99"/>
-      <c r="F19" s="98"/>
+        <v>224</v>
+      </c>
+      <c r="E19" s="95"/>
+      <c r="F19" s="105"/>
       <c r="G19" s="72" t="s">
-        <v>220</v>
-      </c>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
+        <v>219</v>
+      </c>
+      <c r="H19" s="105"/>
+      <c r="I19" s="105"/>
       <c r="J19" s="49"/>
       <c r="K19" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M19" s="28"/>
     </row>
     <row r="20" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A20" s="102"/>
-      <c r="B20" s="102"/>
-      <c r="C20" s="106" t="s">
-        <v>277</v>
+      <c r="A20" s="96"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="109" t="s">
+        <v>276</v>
       </c>
       <c r="D20" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E20" s="102" t="s">
-        <v>257</v>
-      </c>
-      <c r="F20" s="96" t="s">
+        <v>223</v>
+      </c>
+      <c r="E20" s="96" t="s">
+        <v>256</v>
+      </c>
+      <c r="F20" s="94" t="s">
         <v>29</v>
       </c>
       <c r="G20" s="72" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H20" s="66" t="s">
         <v>10</v>
@@ -2971,27 +2971,27 @@
         <v>11</v>
       </c>
       <c r="J20" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="L20" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="K20" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="M20" s="9"/>
     </row>
     <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="102"/>
-      <c r="B21" s="102"/>
-      <c r="C21" s="106"/>
+      <c r="A21" s="96"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="109"/>
       <c r="D21" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E21" s="102"/>
-      <c r="F21" s="97"/>
+        <v>223</v>
+      </c>
+      <c r="E21" s="96"/>
+      <c r="F21" s="104"/>
       <c r="G21" s="72" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H21" s="46" t="s">
         <v>10</v>
@@ -3000,27 +3000,27 @@
         <v>11</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M21" s="9"/>
     </row>
     <row r="22" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="102"/>
-      <c r="B22" s="102"/>
-      <c r="C22" s="106"/>
+      <c r="A22" s="96"/>
+      <c r="B22" s="96"/>
+      <c r="C22" s="109"/>
       <c r="D22" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E22" s="102"/>
-      <c r="F22" s="97"/>
+        <v>223</v>
+      </c>
+      <c r="E22" s="96"/>
+      <c r="F22" s="104"/>
       <c r="G22" s="72" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H22" s="46" t="s">
         <v>10</v>
@@ -3032,24 +3032,24 @@
         <v>71</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="102"/>
-      <c r="B23" s="102"/>
-      <c r="C23" s="106"/>
+      <c r="A23" s="96"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="109"/>
       <c r="D23" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E23" s="102"/>
-      <c r="F23" s="97"/>
+        <v>223</v>
+      </c>
+      <c r="E23" s="96"/>
+      <c r="F23" s="104"/>
       <c r="G23" s="72" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H23" s="46" t="s">
         <v>10</v>
@@ -3061,26 +3061,26 @@
         <v>238</v>
       </c>
       <c r="K23" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="L23" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="L23" s="22" t="s">
-        <v>91</v>
-      </c>
       <c r="M23" s="9"/>
     </row>
     <row r="24" spans="1:13" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="102"/>
-      <c r="B24" s="102"/>
-      <c r="C24" s="106"/>
+      <c r="A24" s="96"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="109"/>
       <c r="D24" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E24" s="102"/>
-      <c r="F24" s="96" t="s">
+        <v>223</v>
+      </c>
+      <c r="E24" s="96"/>
+      <c r="F24" s="94" t="s">
+        <v>277</v>
+      </c>
+      <c r="G24" s="72" t="s">
         <v>278</v>
-      </c>
-      <c r="G24" s="72" t="s">
-        <v>279</v>
       </c>
       <c r="H24" s="46" t="s">
         <v>10</v>
@@ -3089,27 +3089,27 @@
         <v>11</v>
       </c>
       <c r="J24" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="K24" s="18" t="s">
-        <v>82</v>
-      </c>
       <c r="L24" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:13" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="102"/>
-      <c r="B25" s="102"/>
-      <c r="C25" s="106"/>
+      <c r="A25" s="96"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="109"/>
       <c r="D25" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="E25" s="102"/>
-      <c r="F25" s="99"/>
+        <v>223</v>
+      </c>
+      <c r="E25" s="96"/>
+      <c r="F25" s="95"/>
       <c r="G25" s="72" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>10</v>
@@ -3121,121 +3121,133 @@
         <v>72</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M25" s="9"/>
     </row>
     <row r="26" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A26" s="102"/>
-      <c r="B26" s="102"/>
-      <c r="C26" s="106" t="s">
+      <c r="A26" s="96"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="109" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="72" t="s">
-        <v>223</v>
-      </c>
-      <c r="E26" s="102" t="s">
-        <v>176</v>
-      </c>
-      <c r="F26" s="107"/>
+        <v>222</v>
+      </c>
+      <c r="E26" s="96" t="s">
+        <v>175</v>
+      </c>
+      <c r="F26" s="106"/>
       <c r="G26" s="72" t="s">
-        <v>222</v>
-      </c>
-      <c r="H26" s="98" t="s">
+        <v>221</v>
+      </c>
+      <c r="H26" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="98" t="s">
+      <c r="I26" s="105" t="s">
         <v>11</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M26" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="102"/>
-      <c r="B27" s="102"/>
-      <c r="C27" s="106"/>
+      <c r="A27" s="96"/>
+      <c r="B27" s="96"/>
+      <c r="C27" s="109"/>
       <c r="D27" s="72" t="s">
-        <v>223</v>
-      </c>
-      <c r="E27" s="102"/>
-      <c r="F27" s="108"/>
+        <v>222</v>
+      </c>
+      <c r="E27" s="96"/>
+      <c r="F27" s="107"/>
       <c r="G27" s="72" t="s">
-        <v>222</v>
-      </c>
-      <c r="H27" s="98"/>
-      <c r="I27" s="98"/>
+        <v>221</v>
+      </c>
+      <c r="H27" s="105"/>
+      <c r="I27" s="105"/>
       <c r="J27" s="24"/>
       <c r="K27" s="38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M27" s="9"/>
     </row>
     <row r="28" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="102"/>
-      <c r="B28" s="102"/>
-      <c r="C28" s="106"/>
+      <c r="A28" s="96"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="109"/>
       <c r="D28" s="72" t="s">
-        <v>223</v>
-      </c>
-      <c r="E28" s="102"/>
-      <c r="F28" s="108"/>
+        <v>222</v>
+      </c>
+      <c r="E28" s="96"/>
+      <c r="F28" s="107"/>
       <c r="G28" s="72" t="s">
-        <v>222</v>
-      </c>
-      <c r="H28" s="98"/>
-      <c r="I28" s="98"/>
+        <v>221</v>
+      </c>
+      <c r="H28" s="105"/>
+      <c r="I28" s="105"/>
       <c r="J28" s="24"/>
       <c r="K28" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M28" s="9"/>
     </row>
     <row r="29" spans="1:13" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="102"/>
-      <c r="B29" s="102"/>
-      <c r="C29" s="106"/>
+      <c r="A29" s="96"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="109"/>
       <c r="D29" s="72" t="s">
-        <v>223</v>
-      </c>
-      <c r="E29" s="102"/>
-      <c r="F29" s="109"/>
+        <v>222</v>
+      </c>
+      <c r="E29" s="96"/>
+      <c r="F29" s="108"/>
       <c r="G29" s="72" t="s">
-        <v>222</v>
-      </c>
-      <c r="H29" s="98"/>
-      <c r="I29" s="98"/>
+        <v>221</v>
+      </c>
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
       <c r="J29" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="F13:F19"/>
+    <mergeCell ref="C2:C19"/>
+    <mergeCell ref="E2:E19"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="A2:A29"/>
+    <mergeCell ref="B2:B29"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="E20:E25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="E26:E29"/>
     <mergeCell ref="H13:H19"/>
     <mergeCell ref="I13:I19"/>
     <mergeCell ref="F26:F29"/>
@@ -3243,18 +3255,6 @@
     <mergeCell ref="I26:I29"/>
     <mergeCell ref="F20:F23"/>
     <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A2:A29"/>
-    <mergeCell ref="B2:B29"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="E20:E25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="F13:F19"/>
-    <mergeCell ref="C2:C19"/>
-    <mergeCell ref="E2:E19"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="F5:F8"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3315,7 +3315,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K1" s="37" t="s">
         <v>8</v>
@@ -3328,26 +3328,26 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="14" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="97" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="C2" s="94" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="96" t="s">
-        <v>114</v>
-      </c>
       <c r="D2" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="94" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="70" t="s">
         <v>226</v>
-      </c>
-      <c r="E2" s="96" t="s">
-        <v>180</v>
-      </c>
-      <c r="F2" s="96" t="s">
-        <v>181</v>
-      </c>
-      <c r="G2" s="70" t="s">
-        <v>227</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>13</v>
@@ -3357,24 +3357,24 @@
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:13" s="14" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="104"/>
-      <c r="B3" s="104"/>
-      <c r="C3" s="97"/>
+      <c r="A3" s="98"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="104"/>
       <c r="D3" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="70" t="s">
         <v>226</v>
-      </c>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="70" t="s">
-        <v>227</v>
       </c>
       <c r="H3" s="59" t="s">
         <v>13</v>
@@ -3384,24 +3384,24 @@
       </c>
       <c r="J3" s="66"/>
       <c r="K3" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L3" s="66" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" s="14" customFormat="1" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="104"/>
-      <c r="B4" s="104"/>
-      <c r="C4" s="97"/>
+      <c r="A4" s="98"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="104"/>
       <c r="D4" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="70" t="s">
         <v>226</v>
-      </c>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="70" t="s">
-        <v>227</v>
       </c>
       <c r="H4" s="15" t="s">
         <v>10</v>
@@ -3410,27 +3410,27 @@
         <v>11</v>
       </c>
       <c r="J4" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="K4" s="18" t="s">
-        <v>118</v>
-      </c>
       <c r="L4" s="67" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M4" s="26"/>
     </row>
     <row r="5" spans="1:13" s="14" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104"/>
-      <c r="B5" s="104"/>
-      <c r="C5" s="97"/>
+      <c r="A5" s="98"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="104"/>
       <c r="D5" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="70" t="s">
         <v>226</v>
-      </c>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="70" t="s">
-        <v>227</v>
       </c>
       <c r="H5" s="21" t="s">
         <v>10</v>
@@ -3439,27 +3439,27 @@
         <v>11</v>
       </c>
       <c r="J5" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="K5" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="L5" s="87" t="s">
-        <v>88</v>
-      </c>
       <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" s="14" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104"/>
-      <c r="B6" s="104"/>
-      <c r="C6" s="97"/>
+      <c r="A6" s="98"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="104"/>
       <c r="D6" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="70" t="s">
         <v>226</v>
-      </c>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="70" t="s">
-        <v>227</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>10</v>
@@ -3471,24 +3471,24 @@
         <v>216</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:13" s="14" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="97"/>
+      <c r="A7" s="98"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="104"/>
       <c r="D7" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="70" t="s">
         <v>226</v>
-      </c>
-      <c r="E7" s="97"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="70" t="s">
-        <v>227</v>
       </c>
       <c r="H7" s="59" t="s">
         <v>13</v>
@@ -3498,24 +3498,24 @@
       </c>
       <c r="J7" s="58"/>
       <c r="K7" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" s="14" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="97"/>
+      <c r="A8" s="98"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="104"/>
       <c r="D8" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" s="104"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="70" t="s">
         <v>226</v>
-      </c>
-      <c r="E8" s="97"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="70" t="s">
-        <v>227</v>
       </c>
       <c r="H8" s="59" t="s">
         <v>13</v>
@@ -3525,24 +3525,24 @@
       </c>
       <c r="J8" s="59"/>
       <c r="K8" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" s="14" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="104"/>
-      <c r="B9" s="104"/>
-      <c r="C9" s="97"/>
+      <c r="A9" s="98"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="104"/>
       <c r="D9" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="70" t="s">
         <v>226</v>
-      </c>
-      <c r="E9" s="97"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="70" t="s">
-        <v>227</v>
       </c>
       <c r="H9" s="15" t="s">
         <v>10</v>
@@ -3554,26 +3554,26 @@
         <v>225</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="104"/>
-      <c r="B10" s="104"/>
-      <c r="C10" s="97"/>
+      <c r="A10" s="98"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="104"/>
       <c r="D10" s="69" t="s">
-        <v>226</v>
-      </c>
-      <c r="E10" s="97"/>
-      <c r="F10" s="96" t="s">
-        <v>182</v>
+        <v>225</v>
+      </c>
+      <c r="E10" s="104"/>
+      <c r="F10" s="94" t="s">
+        <v>181</v>
       </c>
       <c r="G10" s="70" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H10" s="66" t="s">
         <v>10</v>
@@ -3582,29 +3582,29 @@
         <v>11</v>
       </c>
       <c r="J10" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="L10" s="23" t="s">
         <v>124</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="L10" s="23" t="s">
-        <v>125</v>
       </c>
       <c r="M10" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="104"/>
-      <c r="B11" s="104"/>
-      <c r="C11" s="97"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="104"/>
       <c r="D11" s="69" t="s">
-        <v>226</v>
-      </c>
-      <c r="E11" s="97"/>
-      <c r="F11" s="97"/>
+        <v>225</v>
+      </c>
+      <c r="E11" s="104"/>
+      <c r="F11" s="104"/>
       <c r="G11" s="70" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H11" s="59" t="s">
         <v>13</v>
@@ -3614,24 +3614,24 @@
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M11" s="20"/>
     </row>
     <row r="12" spans="1:13" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="104"/>
-      <c r="B12" s="104"/>
-      <c r="C12" s="97"/>
+      <c r="A12" s="98"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="104"/>
       <c r="D12" s="69" t="s">
-        <v>226</v>
-      </c>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
+        <v>225</v>
+      </c>
+      <c r="E12" s="104"/>
+      <c r="F12" s="104"/>
       <c r="G12" s="70" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H12" s="15" t="s">
         <v>10</v>
@@ -3640,27 +3640,27 @@
         <v>11</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:13" s="14" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A13" s="104"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="97"/>
+      <c r="A13" s="98"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="104"/>
       <c r="D13" s="69" t="s">
-        <v>226</v>
-      </c>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
+        <v>225</v>
+      </c>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
       <c r="G13" s="70" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>10</v>
@@ -3669,27 +3669,27 @@
         <v>11</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="104"/>
-      <c r="B14" s="104"/>
-      <c r="C14" s="97"/>
+      <c r="A14" s="98"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="104"/>
       <c r="D14" s="69" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
+        <v>225</v>
+      </c>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
       <c r="G14" s="70" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H14" s="53" t="s">
         <v>10</v>
@@ -3699,24 +3699,24 @@
       </c>
       <c r="J14" s="9"/>
       <c r="K14" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L14" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:13" s="14" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="104"/>
-      <c r="B15" s="104"/>
-      <c r="C15" s="97"/>
+      <c r="A15" s="98"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="104"/>
       <c r="D15" s="69" t="s">
-        <v>226</v>
-      </c>
-      <c r="E15" s="97"/>
-      <c r="F15" s="99"/>
+        <v>225</v>
+      </c>
+      <c r="E15" s="104"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="70" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>10</v>
@@ -3725,29 +3725,29 @@
         <v>11</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M15" s="9"/>
     </row>
     <row r="16" spans="1:13" s="14" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="104"/>
-      <c r="B16" s="104"/>
-      <c r="C16" s="97"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="104"/>
       <c r="D16" s="69" t="s">
-        <v>226</v>
-      </c>
-      <c r="E16" s="97"/>
-      <c r="F16" s="96" t="s">
-        <v>274</v>
+        <v>225</v>
+      </c>
+      <c r="E16" s="104"/>
+      <c r="F16" s="94" t="s">
+        <v>273</v>
       </c>
       <c r="G16" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H16" s="66" t="s">
         <v>10</v>
@@ -3756,27 +3756,27 @@
         <v>11</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L16" s="67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M16" s="9"/>
     </row>
     <row r="17" spans="1:13" s="14" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="104"/>
-      <c r="B17" s="104"/>
-      <c r="C17" s="97"/>
+      <c r="A17" s="98"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="104"/>
       <c r="D17" s="69" t="s">
-        <v>226</v>
-      </c>
-      <c r="E17" s="97"/>
-      <c r="F17" s="97"/>
+        <v>225</v>
+      </c>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
       <c r="G17" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H17" s="66" t="s">
         <v>10</v>
@@ -3785,27 +3785,27 @@
         <v>11</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L17" s="67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M17" s="9"/>
     </row>
     <row r="18" spans="1:13" s="14" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="104"/>
-      <c r="B18" s="104"/>
-      <c r="C18" s="97"/>
+      <c r="A18" s="98"/>
+      <c r="B18" s="98"/>
+      <c r="C18" s="104"/>
       <c r="D18" s="69" t="s">
-        <v>226</v>
-      </c>
-      <c r="E18" s="97"/>
-      <c r="F18" s="97"/>
+        <v>225</v>
+      </c>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
       <c r="G18" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H18" s="66" t="s">
         <v>10</v>
@@ -3817,24 +3817,24 @@
         <v>35</v>
       </c>
       <c r="K18" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="L18" s="67" t="s">
         <v>140</v>
       </c>
-      <c r="L18" s="67" t="s">
-        <v>141</v>
-      </c>
       <c r="M18" s="9"/>
     </row>
     <row r="19" spans="1:13" s="14" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="104"/>
-      <c r="B19" s="104"/>
-      <c r="C19" s="97"/>
+      <c r="A19" s="98"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="104"/>
       <c r="D19" s="69" t="s">
-        <v>226</v>
-      </c>
-      <c r="E19" s="97"/>
-      <c r="F19" s="97"/>
+        <v>225</v>
+      </c>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
       <c r="G19" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H19" s="66" t="s">
         <v>10</v>
@@ -3844,30 +3844,30 @@
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L19" s="67" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:13" s="84" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="104"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="102" t="s">
-        <v>115</v>
+      <c r="A20" s="98"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="96" t="s">
+        <v>114</v>
       </c>
       <c r="D20" s="70" t="s">
+        <v>229</v>
+      </c>
+      <c r="E20" s="96" t="s">
+        <v>173</v>
+      </c>
+      <c r="F20" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" s="70" t="s">
         <v>230</v>
-      </c>
-      <c r="E20" s="102" t="s">
-        <v>174</v>
-      </c>
-      <c r="F20" s="96" t="s">
-        <v>183</v>
-      </c>
-      <c r="G20" s="70" t="s">
-        <v>231</v>
       </c>
       <c r="H20" s="81" t="s">
         <v>13</v>
@@ -3876,27 +3876,27 @@
         <v>24</v>
       </c>
       <c r="J20" s="82" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L20" s="83" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M20" s="82"/>
     </row>
     <row r="21" spans="1:13" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="104"/>
-      <c r="B21" s="104"/>
-      <c r="C21" s="102"/>
+      <c r="A21" s="98"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="96"/>
       <c r="D21" s="70" t="s">
+        <v>229</v>
+      </c>
+      <c r="E21" s="96"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="70" t="s">
         <v>230</v>
-      </c>
-      <c r="E21" s="102"/>
-      <c r="F21" s="97"/>
-      <c r="G21" s="70" t="s">
-        <v>231</v>
       </c>
       <c r="H21" s="15" t="s">
         <v>13</v>
@@ -3905,27 +3905,27 @@
         <v>24</v>
       </c>
       <c r="J21" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="L21" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="K21" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="L21" s="23" t="s">
-        <v>149</v>
-      </c>
       <c r="M21" s="9"/>
     </row>
     <row r="22" spans="1:13" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="104"/>
-      <c r="B22" s="104"/>
-      <c r="C22" s="102"/>
+      <c r="A22" s="98"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="96"/>
       <c r="D22" s="70" t="s">
+        <v>229</v>
+      </c>
+      <c r="E22" s="96"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="70" t="s">
         <v>230</v>
-      </c>
-      <c r="E22" s="102"/>
-      <c r="F22" s="97"/>
-      <c r="G22" s="70" t="s">
-        <v>231</v>
       </c>
       <c r="H22" s="59" t="s">
         <v>13</v>
@@ -3935,26 +3935,26 @@
       </c>
       <c r="J22" s="24"/>
       <c r="K22" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L22" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:13" s="14" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="104"/>
-      <c r="B23" s="104"/>
-      <c r="C23" s="102"/>
+      <c r="A23" s="98"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="96"/>
       <c r="D23" s="70" t="s">
-        <v>230</v>
-      </c>
-      <c r="E23" s="102"/>
-      <c r="F23" s="98" t="s">
-        <v>172</v>
+        <v>229</v>
+      </c>
+      <c r="E23" s="96"/>
+      <c r="F23" s="105" t="s">
+        <v>171</v>
       </c>
       <c r="G23" s="70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H23" s="66" t="s">
         <v>10</v>
@@ -3964,24 +3964,24 @@
       </c>
       <c r="J23" s="24"/>
       <c r="K23" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L23" s="67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M23" s="9"/>
     </row>
     <row r="24" spans="1:13" s="14" customFormat="1" ht="205.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="104"/>
-      <c r="B24" s="104"/>
-      <c r="C24" s="102"/>
+      <c r="A24" s="98"/>
+      <c r="B24" s="98"/>
+      <c r="C24" s="96"/>
       <c r="D24" s="70" t="s">
-        <v>230</v>
-      </c>
-      <c r="E24" s="102"/>
-      <c r="F24" s="98"/>
+        <v>229</v>
+      </c>
+      <c r="E24" s="96"/>
+      <c r="F24" s="105"/>
       <c r="G24" s="70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H24" s="66" t="s">
         <v>10</v>
@@ -3990,27 +3990,27 @@
         <v>11</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L24" s="67" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M24" s="48"/>
     </row>
     <row r="25" spans="1:13" s="14" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="104"/>
-      <c r="B25" s="104"/>
-      <c r="C25" s="102"/>
+      <c r="A25" s="98"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="96"/>
       <c r="D25" s="70" t="s">
-        <v>230</v>
-      </c>
-      <c r="E25" s="102"/>
-      <c r="F25" s="98"/>
+        <v>229</v>
+      </c>
+      <c r="E25" s="96"/>
+      <c r="F25" s="105"/>
       <c r="G25" s="70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H25" s="66" t="s">
         <v>10</v>
@@ -4019,27 +4019,27 @@
         <v>11</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L25" s="67" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M25" s="48"/>
     </row>
     <row r="26" spans="1:13" s="14" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="104"/>
-      <c r="B26" s="104"/>
-      <c r="C26" s="102"/>
+      <c r="A26" s="98"/>
+      <c r="B26" s="98"/>
+      <c r="C26" s="96"/>
       <c r="D26" s="70" t="s">
-        <v>230</v>
-      </c>
-      <c r="E26" s="102"/>
-      <c r="F26" s="98"/>
+        <v>229</v>
+      </c>
+      <c r="E26" s="96"/>
+      <c r="F26" s="105"/>
       <c r="G26" s="70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H26" s="66" t="s">
         <v>13</v>
@@ -4049,24 +4049,24 @@
       </c>
       <c r="J26" s="24"/>
       <c r="K26" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L26" s="67" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M26" s="48"/>
     </row>
     <row r="27" spans="1:13" s="14" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="104"/>
-      <c r="B27" s="104"/>
-      <c r="C27" s="102"/>
+      <c r="A27" s="98"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="96"/>
       <c r="D27" s="70" t="s">
-        <v>230</v>
-      </c>
-      <c r="E27" s="102"/>
-      <c r="F27" s="98"/>
+        <v>229</v>
+      </c>
+      <c r="E27" s="96"/>
+      <c r="F27" s="105"/>
       <c r="G27" s="70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H27" s="66" t="s">
         <v>13</v>
@@ -4076,26 +4076,26 @@
       </c>
       <c r="J27" s="24"/>
       <c r="K27" s="39" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L27" s="67" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M27" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="F16:F19"/>
     <mergeCell ref="A2:A27"/>
     <mergeCell ref="B2:B27"/>
     <mergeCell ref="C20:C27"/>
     <mergeCell ref="E20:E27"/>
     <mergeCell ref="E2:E19"/>
     <mergeCell ref="C2:C19"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="F2:F9"/>
-    <mergeCell ref="F10:F15"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="F16:F19"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4156,7 +4156,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>8</v>
@@ -4171,19 +4171,19 @@
     </row>
     <row r="2" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="110" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="110"/>
       <c r="C2" s="63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D2" s="68" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E2" s="62"/>
       <c r="F2" s="63"/>
       <c r="G2" s="68" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>13</v>
@@ -4192,13 +4192,13 @@
         <v>24</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L2" s="67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>12</v>
@@ -4209,15 +4209,15 @@
       <c r="A3" s="110"/>
       <c r="B3" s="110"/>
       <c r="C3" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="61" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E3" s="62"/>
       <c r="F3" s="32"/>
       <c r="G3" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>13</v>
@@ -4226,13 +4226,13 @@
         <v>24</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L3" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>12</v>
@@ -4243,19 +4243,19 @@
       <c r="A4" s="110"/>
       <c r="B4" s="110"/>
       <c r="C4" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D4" s="61" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" s="33" t="s">
         <v>237</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>164</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>238</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>10</v>
@@ -4264,13 +4264,13 @@
         <v>11</v>
       </c>
       <c r="J4" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="K4" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="K4" s="29" t="s">
-        <v>153</v>
-      </c>
       <c r="L4" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="28"/>
@@ -4279,17 +4279,17 @@
       <c r="A5" s="110"/>
       <c r="B5" s="110"/>
       <c r="C5" s="113" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D5" s="71" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E5" s="63"/>
       <c r="F5" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G5" s="71" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H5" s="62" t="s">
         <v>10</v>
@@ -4301,10 +4301,10 @@
         <v>33</v>
       </c>
       <c r="K5" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="L5" s="22" t="s">
         <v>268</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>269</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="28"/>
@@ -4314,14 +4314,14 @@
       <c r="B6" s="110"/>
       <c r="C6" s="114"/>
       <c r="D6" s="71" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E6" s="63"/>
       <c r="F6" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G6" s="73" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H6" s="67" t="s">
         <v>10</v>
@@ -4333,7 +4333,7 @@
         <v>34</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>36</v>
@@ -4345,19 +4345,19 @@
       <c r="A7" s="110"/>
       <c r="B7" s="110"/>
       <c r="C7" s="111" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D7" s="112" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="112" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7" s="112" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" s="76" t="s">
         <v>233</v>
-      </c>
-      <c r="E7" s="112" t="s">
-        <v>166</v>
-      </c>
-      <c r="F7" s="112" t="s">
-        <v>158</v>
-      </c>
-      <c r="G7" s="76" t="s">
-        <v>234</v>
       </c>
       <c r="H7" s="74" t="s">
         <v>10</v>
@@ -4367,10 +4367,10 @@
       </c>
       <c r="J7" s="75"/>
       <c r="K7" s="76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L7" s="74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M7" s="75"/>
       <c r="N7" s="7" t="s">
@@ -4385,7 +4385,7 @@
       <c r="E8" s="112"/>
       <c r="F8" s="112"/>
       <c r="G8" s="76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H8" s="77" t="s">
         <v>10</v>
@@ -4395,10 +4395,10 @@
       </c>
       <c r="J8" s="77"/>
       <c r="K8" s="78" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L8" s="79" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M8" s="80"/>
       <c r="N8" s="28"/>
@@ -4420,18 +4420,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4652,26 +4652,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028899C0-A503-43AA-9B4E-6A4DD613BDEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BA4D476-32CA-4B93-8A89-8E5E8618A3F8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="57d38346-cf2b-472c-9a09-6eba75d26f5c"/>
+    <ds:schemaRef ds:uri="9b272e4e-2ce1-4322-a085-a85112500e72"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BA4D476-32CA-4B93-8A89-8E5E8618A3F8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028899C0-A503-43AA-9B4E-6A4DD613BDEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="57d38346-cf2b-472c-9a09-6eba75d26f5c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9b272e4e-2ce1-4322-a085-a85112500e72"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>